<commit_message>
Aula de JS e Ex de C sharp
</commit_message>
<xml_diff>
--- a/ESTUDOS.xlsx
+++ b/ESTUDOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9957488-180D-4E0D-9ECF-3175DBBB7676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608F6DF7-971A-4F24-BDE5-93F79DBBE3AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1640,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9576AA0B-B08B-4420-9211-550F4FC0297A}">
   <dimension ref="B2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="I19" s="7">
         <f>SUM(H19:H22)</f>
-        <v>-0.46527777777777773</v>
+        <v>0.26388888888888901</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="10"/>
@@ -2193,11 +2193,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>0.6875</v>
       </c>
       <c r="H20" s="1">
         <f>G20-F20</f>
-        <v>-0.60416666666666663</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="6"/>
@@ -2221,14 +2221,14 @@
       <c r="D21" s="6"/>
       <c r="E21" s="10"/>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="H21" s="1">
         <f>G21-F21</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="6"/>
@@ -2727,7 +2727,7 @@
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <f>I34+I29+I24+I19+I14+I9+I4+O34+O29+O24+O19+O14+O9+O4</f>
-        <v>-0.13194444444444425</v>
+        <v>0.59722222222222254</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>

</xml_diff>

<commit_message>
Exercicios até dia 08/03/2021
</commit_message>
<xml_diff>
--- a/ESTUDOS.xlsx
+++ b/ESTUDOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB83CD9-14A2-4F2A-8E57-927B9BF44A9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F93F5B1-A9DA-40A4-A17E-432CA95B8536}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="12">
   <si>
     <t>SEGUNDA</t>
   </si>
@@ -1710,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9576AA0B-B08B-4420-9211-550F4FC0297A}">
   <dimension ref="B2:AB39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB40" sqref="A1:AB40"/>
     </sheetView>
   </sheetViews>
@@ -3877,10 +3877,13 @@
   <dimension ref="B2:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
@@ -3966,22 +3969,22 @@
         <v>0.29166666666666657</v>
       </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="6" t="s">
-        <v>9</v>
+      <c r="K4" s="6">
+        <v>44263</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N4" s="1">
         <f>M4-L4</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="O4" s="9">
         <f>SUM(N4:N7)</f>
-        <v>0</v>
+        <v>0.25694444444444442</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="6" t="s">
@@ -4040,14 +4043,14 @@
       <c r="J5" s="8"/>
       <c r="K5" s="6"/>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="N5" s="1">
         <f>M5-L5</f>
-        <v>0</v>
+        <v>0.13194444444444442</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
@@ -5862,7 +5865,7 @@
     <row r="38" spans="2:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <f>SUM(I34,I29,I24,I19,I14,I9,I4,O4,O9,O14,O19,O24,O29,O34)</f>
-        <v>0.77083333333333304</v>
+        <v>1.0277777777777775</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -5871,7 +5874,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="14">
-        <f>SUM(I34,I29,I24,I19,I14,I9,I4)</f>
+        <f>SUM(I19,I4,I9,I14,I24,I29,I34)</f>
         <v>0.77083333333333304</v>
       </c>
       <c r="J38" s="4"/>
@@ -5880,8 +5883,8 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="14">
-        <f>SUM(O34,O29,O24,O19,O14,O9,O4)</f>
-        <v>0</v>
+        <f>SUM(O19,O4,O9,O14,O24,O29,O34)</f>
+        <v>0.25694444444444442</v>
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="5"/>

</xml_diff>